<commit_message>
Change xls files Headers
</commit_message>
<xml_diff>
--- a/contacts-with-errors.xlsx
+++ b/contacts-with-errors.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">Full Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
   </si>
   <si>
     <t xml:space="preserve">sdfsd</t>
@@ -169,10 +169,10 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>

</xml_diff>